<commit_message>
excel import basic feature added
</commit_message>
<xml_diff>
--- a/public/js/xlsx/list_of_evaluers.xlsx
+++ b/public/js/xlsx/list_of_evaluers.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>maxime.fontanille@gmail.com</t>
   </si>
@@ -83,6 +84,126 @@
   </si>
   <si>
     <t>department</t>
+  </si>
+  <si>
+    <t>Nataliya</t>
+  </si>
+  <si>
+    <t>Nata INC</t>
+  </si>
+  <si>
+    <t>nata@fontanille.com</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Aussenac</t>
+  </si>
+  <si>
+    <t>Jean-Christophe</t>
+  </si>
+  <si>
+    <t>Bouvier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuel </t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurelie </t>
+  </si>
+  <si>
+    <t>Lejeune</t>
+  </si>
+  <si>
+    <t>Yoann</t>
+  </si>
+  <si>
+    <t>Garnier</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Cox</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Guetta</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>En Pure</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>Prodigy</t>
+  </si>
+  <si>
+    <t>Chemical</t>
+  </si>
+  <si>
+    <t>Brothers</t>
+  </si>
+  <si>
+    <t>Freelancer</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>freelancer@gmail.com</t>
+  </si>
+  <si>
+    <t>john@yies.co</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doo</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Dupont</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>YIES</t>
+  </si>
+  <si>
+    <t>laura@ibm.fr</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Sales Manager</t>
+  </si>
+  <si>
+    <t>nicolas@nike.no</t>
   </si>
 </sst>
 </file>
@@ -447,7 +568,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,40 +662,236 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -587,8 +904,113 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed error in NE3
</commit_message>
<xml_diff>
--- a/public/js/xlsx/list_of_evaluers.xlsx
+++ b/public/js/xlsx/list_of_evaluers.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
   <si>
     <t>maxime.fontanille@gmail.com</t>
   </si>
@@ -162,48 +161,6 @@
   </si>
   <si>
     <t>freelancer@gmail.com</t>
-  </si>
-  <si>
-    <t>john@yies.co</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doo</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>Williams</t>
-  </si>
-  <si>
-    <t>Dupont</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
-    <t>YIES</t>
-  </si>
-  <si>
-    <t>laura@ibm.fr</t>
-  </si>
-  <si>
-    <t>IBM</t>
-  </si>
-  <si>
-    <t>Nike</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Sales Manager</t>
-  </si>
-  <si>
-    <t>nicolas@nike.no</t>
   </si>
 </sst>
 </file>
@@ -568,7 +525,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,107 +867,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>